<commit_message>
Added section where COVID revenue from fed gov is dropped to better assess fiscal gap.
</commit_message>
<xml_diff>
--- a/ioc_source_updated22_AWM.xlsx
+++ b/ioc_source_updated22_AWM.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Desktop\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D563857F-CD15-4D7D-9C20-4F774DC73358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C02C17F-13AE-4645-983E-90606A956F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="366" yWindow="366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11544" yWindow="4500" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="rev source key" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="8" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9659" uniqueCount="4789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9789" uniqueCount="4810">
   <si>
     <t>source</t>
   </si>
@@ -14306,9 +14309,6 @@
     <t>INDIVIDUAL INCOME TAXES, gross of local, net of refunds</t>
   </si>
   <si>
-    <t>FEDERAL OTHER</t>
-  </si>
-  <si>
     <t>FEDERAL MEDICAID</t>
   </si>
   <si>
@@ -14327,9 +14327,6 @@
     <t>RECEIPTS FROM REVENUE PRODUCNG</t>
   </si>
   <si>
-    <t>ALL OTHER SOURCES</t>
-  </si>
-  <si>
     <t>LICENSES, FEES &amp; REGISTRATIONS</t>
   </si>
   <si>
@@ -14400,6 +14397,75 @@
   </si>
   <si>
     <t>ENRGY TRANSITION ASST/ELECTRIC</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Medical Cannabis</t>
+  </si>
+  <si>
+    <t>Recreational Cannabis</t>
+  </si>
+  <si>
+    <t>Horse Racing Taxes &amp; Fees</t>
+  </si>
+  <si>
+    <t>Garnishment-Levies</t>
+  </si>
+  <si>
+    <t>Student Fees-Universities</t>
+  </si>
+  <si>
+    <t>Retirement Contributions</t>
+  </si>
+  <si>
+    <t>Federal Sources (Other)</t>
+  </si>
+  <si>
+    <t>Investment Income</t>
+  </si>
+  <si>
+    <t>Other Grants and Contracts</t>
+  </si>
+  <si>
+    <t>Proceeds, investment maturities</t>
+  </si>
+  <si>
+    <t>Bond Issue Proceeds</t>
+  </si>
+  <si>
+    <t>Inter-agency Receipts</t>
+  </si>
+  <si>
+    <t>All Other Sources</t>
+  </si>
+  <si>
+    <t>Cook County IGT</t>
+  </si>
+  <si>
+    <t>Short-term Borrowing</t>
+  </si>
+  <si>
+    <t>Prior Year Refunds</t>
+  </si>
+  <si>
+    <t>Statutory Transfers</t>
+  </si>
+  <si>
+    <t>included</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -14437,11 +14503,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14457,6 +14533,573 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alea Wilbur" refreshedDate="44883.559195601854" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="37" xr:uid="{F1ECC298-F13F-4381-8BF1-314BF781B99D}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C38" sheet="rev source key"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="rev_type" numFmtId="49">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="28" maxValue="85" count="37">
+        <s v="02"/>
+        <s v="03"/>
+        <s v="06"/>
+        <s v="09"/>
+        <s v="12"/>
+        <s v="15"/>
+        <s v="18"/>
+        <s v="21"/>
+        <s v="24"/>
+        <s v="27"/>
+        <n v="28"/>
+        <n v="29"/>
+        <n v="30"/>
+        <s v="31"/>
+        <n v="32"/>
+        <s v="33"/>
+        <s v="35"/>
+        <s v="36"/>
+        <s v="39"/>
+        <s v="42"/>
+        <n v="45"/>
+        <s v="48"/>
+        <n v="51"/>
+        <s v="54"/>
+        <s v="57"/>
+        <s v="58"/>
+        <s v="59"/>
+        <n v="60"/>
+        <n v="63"/>
+        <s v="66"/>
+        <s v="72"/>
+        <s v="75"/>
+        <s v="78"/>
+        <s v="79"/>
+        <n v="85"/>
+        <s v="98"/>
+        <s v="99"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="rev_type_name" numFmtId="0">
+      <sharedItems count="37">
+        <s v="INDIVIDUAL INCOME TAXES, gross of local, net of refunds"/>
+        <s v="CORPORATE INCOME TAXES, gross of PPRT, net of refunds"/>
+        <s v="SALES TAXES, gross of local share"/>
+        <s v="MOTOR FUEL TAX, gross of local share, net of refunds"/>
+        <s v="PUBLIC UTILITY TAXES, gross of PPRT"/>
+        <s v="CIGARETTE TAXES"/>
+        <s v="LIQUOR GALLONAGE TAXES"/>
+        <s v="INHERITANCE TAX"/>
+        <s v="INSURANCE TAXES&amp;FEES&amp;LICENSES, net of refunds "/>
+        <s v="CORP FRANCHISE TAXES &amp; FEES"/>
+        <s v="Medical Cannabis"/>
+        <s v="Recreational Cannabis"/>
+        <s v="Horse Racing Taxes &amp; Fees"/>
+        <s v="MEDICAL PROVIDER ASSESSMENTS"/>
+        <s v="Garnishment-Levies"/>
+        <s v="LOTTERY RECEIPTS"/>
+        <s v="OTHER TAXES"/>
+        <s v="RECEIPTS FROM REVENUE PRODUCNG"/>
+        <s v="LICENSES, FEES &amp; REGISTRATIONS"/>
+        <s v="MOTOR VEHICLE AND OPERATORS"/>
+        <s v="Student Fees-Universities"/>
+        <s v="RIVERBOAT WAGERING TAXES"/>
+        <s v="Retirement Contributions"/>
+        <s v="GIFTS AND BEQUESTS"/>
+        <s v="Federal Sources (Other)"/>
+        <s v="FEDERAL MEDICAID"/>
+        <s v="FEDERAL TRANSPORTATION"/>
+        <s v="Other Grants and Contracts"/>
+        <s v="Investment Income"/>
+        <s v="Proceeds, investment maturities"/>
+        <s v="Bond Issue Proceeds"/>
+        <s v="Inter-agency Receipts"/>
+        <s v="All Other Sources"/>
+        <s v="Cook County IGT"/>
+        <s v="Short-term Borrowing"/>
+        <s v="Prior Year Refunds"/>
+        <s v="Statutory Transfers"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="included" numFmtId="0">
+      <sharedItems count="2">
+        <s v="yes"/>
+        <s v="no"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="37">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="15"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="17"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="18"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="19"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="20"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="23"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="24"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="25"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="26"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="27"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="28"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="29"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="30"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="31"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="32"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="33"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="34"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="35"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="36"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49EEBAE8-29F6-463B-9B2F-33AF9E80ABD6}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E1:F41" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="37">
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="14"/>
+        <item x="20"/>
+        <item x="22"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="34"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="35"/>
+        <item x="36"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="38">
+        <item x="32"/>
+        <item x="30"/>
+        <item x="5"/>
+        <item x="33"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="26"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="31"/>
+        <item x="28"/>
+        <item x="18"/>
+        <item x="6"/>
+        <item x="15"/>
+        <item x="10"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="16"/>
+        <item x="35"/>
+        <item x="29"/>
+        <item x="4"/>
+        <item x="17"/>
+        <item x="11"/>
+        <item x="22"/>
+        <item x="21"/>
+        <item x="2"/>
+        <item x="34"/>
+        <item x="36"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="40">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="35"/>
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+      <x v="32"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="33"/>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14777,7 +15420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2370" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B2375" sqref="B2375"/>
     </sheetView>
   </sheetViews>
@@ -49057,7 +49700,7 @@
         <v>2737</v>
       </c>
       <c r="B2372" t="s">
-        <v>4779</v>
+        <v>4777</v>
       </c>
     </row>
     <row r="2373" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49065,7 +49708,7 @@
         <v>2738</v>
       </c>
       <c r="B2373" t="s">
-        <v>4780</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="2374" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49073,7 +49716,7 @@
         <v>2739</v>
       </c>
       <c r="B2374" s="1" t="s">
-        <v>4781</v>
+        <v>4779</v>
       </c>
     </row>
     <row r="2375" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49081,7 +49724,7 @@
         <v>2740</v>
       </c>
       <c r="B2375" s="1" t="s">
-        <v>4788</v>
+        <v>4786</v>
       </c>
     </row>
     <row r="2376" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49089,7 +49732,7 @@
         <v>2742</v>
       </c>
       <c r="B2376" s="1" t="s">
-        <v>4787</v>
+        <v>4785</v>
       </c>
     </row>
     <row r="2377" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49097,7 +49740,7 @@
         <v>2745</v>
       </c>
       <c r="B2377" s="1" t="s">
-        <v>4786</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="2378" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49105,7 +49748,7 @@
         <v>2747</v>
       </c>
       <c r="B2378" s="1" t="s">
-        <v>4785</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="2379" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49113,7 +49756,7 @@
         <v>2748</v>
       </c>
       <c r="B2379" s="1" t="s">
-        <v>4784</v>
+        <v>4782</v>
       </c>
     </row>
     <row r="2380" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49121,7 +49764,7 @@
         <v>2755</v>
       </c>
       <c r="B2380" s="1" t="s">
-        <v>4783</v>
+        <v>4781</v>
       </c>
     </row>
     <row r="2381" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49129,7 +49772,7 @@
         <v>2756</v>
       </c>
       <c r="B2381" s="1" t="s">
-        <v>4782</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="2382" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -49555,200 +50198,686 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C7C91E-452A-4790-95AC-69435DD900FB}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.83984375" style="3"/>
+    <col min="2" max="2" width="43.62890625" customWidth="1"/>
+    <col min="5" max="5" width="12.05078125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.7890625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>4718</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4751</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>4806</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4787</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
         <v>4719</v>
       </c>
       <c r="B2" t="s">
         <v>4756</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>4720</v>
       </c>
       <c r="B3" t="s">
+        <v>4759</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E3" s="6">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>4721</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4758</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E4" s="6">
+        <v>45</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>4722</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4761</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E5" s="6">
+        <v>51</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>4723</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4767</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E6" s="6">
+        <v>85</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>4803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>4724</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4769</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4740</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>4764</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
+        <v>4725</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4772</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4744</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>4798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>4726</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4745</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>4727</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4771</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>4746</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>4728</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4774</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>4748</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4789</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>4749</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4790</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4750</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4791</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3" t="s">
+        <v>4731</v>
+      </c>
+      <c r="B15" t="s">
         <v>4760</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>4721</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>4722</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4762</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>4723</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4769</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>4724</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4771</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>4725</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4774</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>4726</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4772</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>4727</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4773</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>4728</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4776</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>4731</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4761</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="C15" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E15" s="6">
+        <v>28</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>4789</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4792</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E16" s="6">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
         <v>4733</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4770</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>4734</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4710</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>4735</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4763</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>4729</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4765</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>4736</v>
       </c>
       <c r="B17" t="s">
         <v>4768</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+      <c r="C17" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E17" s="6">
+        <v>30</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>4791</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>4734</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4710</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E18" s="6">
+        <v>60</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
+        <v>4735</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4762</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E19" s="6">
+        <v>63</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3" t="s">
+        <v>4729</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4763</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4719</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
+        <v>4736</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4766</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>4720</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4793</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>4721</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
         <v>4738</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B23" t="s">
+        <v>4773</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>4722</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4794</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>4723</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3" t="s">
+        <v>4740</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4764</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4808</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4809</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>4724</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3" t="s">
+        <v>4741</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4795</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>4725</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>4772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3" t="s">
         <v>4775</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>4740</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B27" t="s">
+        <v>4757</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>4726</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="3" t="s">
+        <v>4776</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4765</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>4727</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="3">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4797</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>4728</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4796</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>4731</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="7" t="s">
+        <v>4744</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4798</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>4733</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7" t="s">
+        <v>4745</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4799</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>4734</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="7" t="s">
+        <v>4746</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4800</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>4735</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="7" t="s">
+        <v>4747</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4801</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4807</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>4729</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="7" t="s">
+        <v>4748</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4802</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>4736</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>4766</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="7">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4803</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>4738</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="7" t="s">
+        <v>4749</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4804</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>4741</v>
       </c>
-      <c r="B20" t="s">
+      <c r="F37" s="5" t="s">
+        <v>4795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="7" t="s">
+        <v>4750</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4805</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4808</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>4775</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>4757</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>4777</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4758</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>4778</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4767</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E39" s="6" t="s">
+        <v>4776</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E40" s="6" t="s">
         <v>4747</v>
       </c>
-      <c r="B23" t="s">
-        <v>4764</v>
+      <c r="F40" s="5" t="s">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E41" s="5" t="s">
+        <v>4788</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>